<commit_message>
Edit make excel | Add goods gridView | Final version 1.1
</commit_message>
<xml_diff>
--- a/Отчет.xlsx
+++ b/Отчет.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Soft\workspace\RadProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD9D67D-BD0D-4836-86BE-3493DA4BBE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58CBF74-5B50-4CFB-A0EB-7EC7DC5F6A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="2355" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Номер контракта</t>
-  </si>
-  <si>
-    <t>Имя</t>
-  </si>
-  <si>
-    <t>Фамилия</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Название товара</t>
   </si>
@@ -45,28 +36,16 @@
     <t>Сумма</t>
   </si>
   <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>Shirko</t>
-  </si>
-  <si>
     <t>Таблетки</t>
   </si>
   <si>
     <t>Место в культе дружбы</t>
   </si>
   <si>
-    <t>Semen</t>
-  </si>
-  <si>
-    <t>Mahal</t>
+    <t>Шаурма с солями</t>
   </si>
   <si>
     <t>Урматы</t>
-  </si>
-  <si>
-    <t>Шаурма с солями</t>
   </si>
 </sst>
 </file>
@@ -384,21 +363,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,94 +379,49 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1560</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="B5">
         <v>2</v>
       </c>
-      <c r="F2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
+      <c r="C5">
         <v>201000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>1560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>